<commit_message>
[MOSIP-19230] Virtual machine type and spec added.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/xlsx/machine_spec.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/xlsx/machine_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -47,15 +47,31 @@
   </si>
   <si>
     <t xml:space="preserve">is_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RESIDENT-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident Virtual Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENT-REG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -137,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +164,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -167,13 +187,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576 1:1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.02"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -202,6 +233,35 @@
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>